<commit_message>
finishes with all comments in excel file and changes to Plagiarism project
</commit_message>
<xml_diff>
--- a/Plagiarism-f17-imSlow/inefficiencies.xlsx
+++ b/Plagiarism-f17-imSlow/inefficiencies.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>Your name:</t>
   </si>
@@ -77,44 +77,296 @@
     <t>119.6034 seconds (avg. over 5 trials)</t>
   </si>
   <si>
-    <t>readFile()</t>
-  </si>
-  <si>
     <t xml:space="preserve">code is redundant-- file is read and every word is stored with this method, only to be read over again to create phrases in createPhrases(). </t>
   </si>
   <si>
-    <t>eliminate the extra work all together -- take the window value into account from the beginning and read the file only once to create a list of phrases of size window.</t>
-  </si>
-  <si>
     <t>findMatches()</t>
   </si>
   <si>
     <t>detectPlagiarism()</t>
   </si>
   <si>
-    <t>sortResults()</t>
-  </si>
-  <si>
-    <t>Does a lot of work that can be totally replaced with a more appropriate data structure.</t>
-  </si>
-  <si>
-    <t>Changed the data structure for the matches and filenames to a TreeMap (Key- match #, value - filename), and took advantage of the fact that a TreeMap has the ability to be reverse sorted built in already.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First of all there is a nested for loop in which a file is compared to all other files by created phrase lists for each file and then a set is formed of all the matching phrases between the two file. First off, this method doesn't account for the file being compared to itself, which is wasted time and resources. Secondly, these phrase lists are generated EACH TIME the method is run i.e. n^2 times. </t>
-  </si>
-  <si>
     <t>There is a lot of unnecessary work being done in this method. The nested for loop is a good place to start, as each of 'my' phrases are compared to each of 'your' phrases. This could be sped up by just interating over 1 list of phrases and if the other persons list contains it add it to the set and then break. There's no need to keep comparing the matching phrase to the remaining phrases in the other list. More importantly, this method is wasting a lot of space by storing all the matching phrases in a set, when in all reality all this method needs to return is an int of the number of matches.</t>
   </si>
   <si>
-    <t>Instead of using a set I changed matches to be an int. I also made copies of the phrases, so when comparing phrases I could eliminate matching phrases when encountered.</t>
+    <t xml:space="preserve">First of all there is a nested for loop in which a file is compared to all other files by created phrase lists for each file and then a set is formed of all the matching phrases between the two file. Secondly, these phrase lists are generated EACH TIME the method is run i.e. n^2 times. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another major inefficiency of this method is that it doesn't account for the file being compared to itself, or file A being compared to file B, and later file B being compared to file A, which are both wasted time and resources. </t>
+  </si>
+  <si>
+    <t>createPhrases/readFile(eliminated)</t>
+  </si>
+  <si>
+    <t>it created a giant list of all words for each file, only to iterate over that list to get a list of phrases</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">M2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>- Instead of a nested for loop that iterates over all phrases in file 2 while iterating over all phrases in file 1, I just iterate over file 1 ('myPhrases'), and if file 2 ('yourPhrases') contains the current phrase then increase the match count. (line 73-79)</t>
+    </r>
+  </si>
+  <si>
+    <t>readFile()/createPhrases()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>M1-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> I eliminated the extra work of creating a word list first all together -- I took the window value into account from the beginning and read the file only once to create a list of phrases of size window. (Lines 26-61)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>M3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - (line 98) - moved the createPhrase() method into the outer for loop, so it is only done i many times as opposed to i x j many times. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>M4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - (line 105) - only process file 2 if it's different from file 1, and if it hasn't already been compared to file 1.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">avg: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>6.8462 seconds over 5 trials</t>
+    </r>
+  </si>
+  <si>
+    <t>createPhrases()</t>
+  </si>
+  <si>
+    <t>It's changing input to all uppercase, though the majority of the letters will be lowercase.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>m1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> - in addition to the two methods being combined, a word list of size #window is created, then changed to a string and stored as a phrase, before the 0th index element is eliminated and the next word is added at the end. At that point the list enters the phrase creation loop again. This way a word list of only size #window is maintained during the creation of the phrase list as opposed to one the size of all the words in the text(s).  (line 39-53)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m2 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>I changed the method to toLowerCase() so less swapping would need to be done. (line 41)</t>
+    </r>
+  </si>
+  <si>
+    <t>detectPlagiarism()/ sortResults()</t>
+  </si>
+  <si>
+    <t>Does a lot of work that can (possibly) be improved with a more appropriate data structure.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m10 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Changed the data structure for the matches and filenames to a TreeMap (Key- match #, value - filename), and took advantage of the fact that a TreeMap has the ability to be reverse sorted built in already. However, then realized that the problem would be with repeat keys, so I opted to keep the prior storage (key - filename, value - int number of matches), and looked for a more efficient way to sort by value.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m3 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>I was originally using a separate data structure (ArrayList) to build/store the individual phrases, but then realized I could eliminate the structure all together and just used the 'words' ArrayList to create the individual phrases. (lines 43-46)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Originally the class was using a string to build each individual phrase, which was inefficient due to the fact that strings are immutable in Java. </t>
+  </si>
+  <si>
+    <r>
+      <t>m4 -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (line 49 -51) I commented out the check to see if the phrase was already present -- given that we are using a hashset data structure if we try and store a repeat value the repeat instance won't be stored (check not needed). </t>
+    </r>
+  </si>
+  <si>
+    <t>The code checks to see if a phrase is present in hashset of all phrases before storing it.</t>
+  </si>
+  <si>
+    <t>Method has a for loop to iterate over all my phrases and a nested for loop to iterate over all your phrases.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m5 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>In addition to getting rid of the nested for loop I also made a copy of 'yourPhrases' (a memory tradeoff), and then proceeded to remove matching phrases from this copy hashset in hope of improving performance in files with large amounts of matches. (line 69-79)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Method storing matches as a set of strings only to use its size later. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m6 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(line 67-81) changed the return type of method to int, thus freeing up memory space.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m7 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(lines 102-103) moved both equivalent comparisons/filenames (file1+"-"+file2 / file2+"-"+file1) outside of the primary loop so as to catch any repetition BEFORE any repeat comparisons would be done -- this way if the two files were already compared a list of phrases for one file would never be created and the method to find the matches would never be called.</t>
+    </r>
+  </si>
+  <si>
+    <t>The method only catches repeat comparisons (file1-to-file2 &amp; file2-to-file1) as well as comparsions of a file to itself AFTER all the processing of the files has been completed (lines 112-115). All this is really doing is preventing the results from being printed, not the work from being done in the first place.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is an unnecessary condition check that would be handled before (redundant). </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m8 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>Commented out the check to see if matches was null (line 111)</t>
+    </r>
+  </si>
+  <si>
+    <t>Checked condition to see if file was compared to itself is no longer needed due to method refactoring.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">m9 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>(line 113-114) modified to only check if an instance of the files comparison is present in the list.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +401,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -173,7 +437,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -194,8 +458,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -222,8 +488,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="19" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -233,6 +504,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -580,12 +853,12 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
     <col min="2" max="2" width="43.5" style="4" customWidth="1"/>
     <col min="3" max="3" width="61.33203125" style="4" customWidth="1"/>
   </cols>
@@ -657,56 +930,58 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="2" customFormat="1" ht="208" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="2" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C13" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="2" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -717,39 +992,115 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="6"/>
+    <row r="16" spans="1:3" s="2" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="6"/>
+      <c r="A21" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="3" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="6"/>
+      <c r="A23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="6"/>
+      <c r="A24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="3" customFormat="1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
@@ -773,7 +1124,9 @@
       <c r="A29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>